<commit_message>
done w recycle bin; do not touch
</commit_message>
<xml_diff>
--- a/TMS/public/csv/Journal-Entry-template.xlsx
+++ b/TMS/public/csv/Journal-Entry-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\AIMS-Capstone\TMS\public\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6650246-D0C0-44E1-AA21-D467F64FC841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3ACF77-0C2A-49F6-AFE4-8DFDB083EFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D031EBA5-5603-4D96-9A32-9227E196D84B}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{D031EBA5-5603-4D96-9A32-9227E196D84B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -448,7 +448,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>2500</v>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="D3">
-        <v>1010</v>
+        <v>501</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -488,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>1500</v>
+        <v>160</v>
       </c>
       <c r="E4">
         <v>4000</v>
@@ -508,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>2500</v>
+        <v>314</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -531,6 +531,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D043D0F840028B4FA33DA8E91EC0A5AE" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="91fdc9c771a7089613324da7b6009805">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c461d7d0-a753-4715-b08d-465ab101aa23" xmlns:ns4="b582f8a7-63d8-4bf6-af4a-67681bfed095" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8ac4d9a94d92ab4ac184bf52c570f953" ns3:_="" ns4:_="">
     <xsd:import namespace="c461d7d0-a753-4715-b08d-465ab101aa23"/>
@@ -763,15 +772,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A977E8D-C2AE-4B3B-B87A-88F58A717632}">
   <ds:schemaRefs>
@@ -790,6 +790,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B4F361-51AE-4C2D-BE1E-05CC02F68016}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71CE5EA3-EB9D-4B27-A444-F93C75A40F61}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -806,12 +814,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53B4F361-51AE-4C2D-BE1E-05CC02F68016}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>